<commit_message>
inventory adn sales paeg updated , daybook
</commit_message>
<xml_diff>
--- a/Reference data/SALESMAN TEMPLATE.xlsx
+++ b/Reference data/SALESMAN TEMPLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Distribution Software\Reference data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62F89497-5104-42AE-B25C-F5A48897AE96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A42F238-ADB5-49ED-AF3B-FDAD89C79A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D9D52DD1-4413-4DC5-B3B5-199C8E01F75E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t xml:space="preserve">        Date:-</t>
   </si>
@@ -190,6 +190,33 @@
   </si>
   <si>
     <t>FUEL PRICE DIFFER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPENING </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLOSING </t>
+  </si>
+  <si>
+    <t>CRAFTED Foils</t>
+  </si>
+  <si>
+    <t>WHOLESALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRAFTED SCHEME </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZYN </t>
+  </si>
+  <si>
+    <t>TK REWARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANK TRANSFER </t>
+  </si>
+  <si>
+    <t>EXPENSES DETAILS:</t>
   </si>
 </sst>
 </file>
@@ -197,8 +224,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -294,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +384,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,14 +581,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -562,16 +604,16 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -580,22 +622,13 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -642,15 +675,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -658,6 +703,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -667,10 +734,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="165" formatCode="\-\-\-"/>
+      <numFmt numFmtId="166" formatCode="\-\-\-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="\-"/>
+      <numFmt numFmtId="167" formatCode="\-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -982,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6782F9B3-8001-4925-B919-A9A83F4471B2}">
-  <dimension ref="B1:J35"/>
+  <dimension ref="B1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29:M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,588 +1065,668 @@
     <col min="7" max="7" width="23.5703125" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="13" width="25.140625" customWidth="1"/>
+    <col min="14" max="14" width="2.140625" style="58" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" ht="21" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="45">
         <v>45808</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-    </row>
-    <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="9">
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
         <f t="shared" ref="B3:B19" si="0">C3*D3</f>
         <v>28925</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <f t="shared" ref="D3:D19" si="1">F3-E3</f>
         <v>2.5</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>2.5</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>5</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B4" s="9">
+    <row r="4" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B4" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>1</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>1</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
+    <row r="5" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B5" s="8">
         <f t="shared" si="0"/>
         <v>1804.1999999999996</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <f t="shared" si="1"/>
         <v>0.19999999999999996</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>0.8</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>1</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
+    <row r="6" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
         <f t="shared" si="0"/>
         <v>9527</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="10">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E6" s="12">
-        <v>0</v>
-      </c>
-      <c r="F6" s="12">
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11">
         <v>1</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="G6" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
+    <row r="7" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>26865</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>0.2</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>0.2</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B8" s="9">
+    <row r="8" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>0.4</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>0.4</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B9" s="9">
+    <row r="9" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15" t="s">
+      <c r="E9" s="11"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
+    <row r="10" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="16" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="B11" s="9">
+    <row r="11" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="16" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="B12" s="9">
+    <row r="12" spans="2:16" ht="21" x14ac:dyDescent="0.3">
+      <c r="B12" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="16" t="s">
+      <c r="E12" s="11"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="B13" s="9">
+    <row r="13" spans="2:16" ht="21" x14ac:dyDescent="0.3">
+      <c r="B13" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="16" t="s">
+      <c r="E13" s="11"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="B14" s="9">
+    <row r="14" spans="2:16" ht="21" x14ac:dyDescent="0.3">
+      <c r="B14" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="16" t="s">
+      <c r="E14" s="11"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="B15" s="9">
+    <row r="15" spans="2:16" ht="21" x14ac:dyDescent="0.3">
+      <c r="B15" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="15" t="s">
+      <c r="E15" s="11"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="21" x14ac:dyDescent="0.3">
-      <c r="B16" s="9">
+    <row r="16" spans="2:16" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="16" t="s">
+      <c r="E16" s="11"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" ht="21" x14ac:dyDescent="0.3">
-      <c r="B17" s="9">
+      <c r="L16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="M16" s="9"/>
+      <c r="O16" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" s="55"/>
+    </row>
+    <row r="17" spans="2:16" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="16" t="s">
+      <c r="E17" s="11"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" ht="21" x14ac:dyDescent="0.3">
-      <c r="B18" s="9">
+      <c r="L17" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="59"/>
+      <c r="O17" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="P17" s="53">
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="16" t="s">
+      <c r="E18" s="11"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" ht="21" x14ac:dyDescent="0.3">
-      <c r="B19" s="9">
+      <c r="L18" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="M18" s="9"/>
+      <c r="O18" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="P18" s="53">
+        <v>2293</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="15" t="s">
+      <c r="E19" s="11"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" ht="21" x14ac:dyDescent="0.3">
-      <c r="B20" s="9">
+      <c r="L19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M19" s="9"/>
+      <c r="O19" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="P19" s="57">
+        <f>(P18-P17)*5.5</f>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="8">
         <f>SUM(B3:B19)</f>
         <v>40256.199999999997</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="17">
         <f>SUM(D3:D19)</f>
         <v>3.7</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="17">
         <f>SUM(E3:E19)</f>
         <v>4.9000000000000004</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="17">
         <f>SUM(F3:F19)</f>
         <v>8.6</v>
       </c>
-      <c r="G20" s="19"/>
-    </row>
-    <row r="21" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B21" s="20">
+      <c r="G20" s="18"/>
+      <c r="L20" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M20" s="9"/>
+      <c r="O20" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="P20" s="54"/>
+    </row>
+    <row r="21" spans="2:16" ht="26.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="19">
         <v>307</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22" t="s">
+      <c r="D21" s="20"/>
+      <c r="E21" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
-    </row>
-    <row r="22" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B22" s="25"/>
-      <c r="C22" s="26" t="s">
+      <c r="F21" s="47"/>
+      <c r="G21" s="48"/>
+      <c r="L21" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="M21" s="9"/>
+    </row>
+    <row r="22" spans="2:16" ht="26.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="21"/>
+      <c r="C22" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="27">
+      <c r="D22" s="20"/>
+      <c r="E22" s="23">
         <v>5000</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="8">
         <v>1</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="8">
         <f>E22*F22</f>
         <v>5000</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B23" s="25"/>
-      <c r="C23" s="13" t="s">
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+    </row>
+    <row r="23" spans="2:16" ht="26.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="21"/>
+      <c r="C23" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="29">
+      <c r="D23" s="24"/>
+      <c r="E23" s="25">
         <v>1000</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F23" s="26">
         <v>27</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="8">
         <f t="shared" ref="G23:G28" si="2">E23*F23</f>
         <v>27000</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" ht="21" x14ac:dyDescent="0.3">
-      <c r="B24" s="25"/>
-      <c r="C24" s="13" t="s">
+      <c r="L23" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M23" s="9"/>
+    </row>
+    <row r="24" spans="2:16" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="21"/>
+      <c r="C24" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="31"/>
-      <c r="E24" s="9">
+      <c r="D24" s="27"/>
+      <c r="E24" s="8">
         <v>500</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F24" s="25">
         <v>15</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="8">
         <f t="shared" si="2"/>
         <v>7500</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" ht="21" x14ac:dyDescent="0.3">
-      <c r="B25" s="25"/>
-      <c r="C25" s="13" t="s">
+      <c r="L24" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="M24" s="9"/>
+    </row>
+    <row r="25" spans="2:16" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="21"/>
+      <c r="C25" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="32"/>
-      <c r="E25" s="33">
+      <c r="D25" s="28"/>
+      <c r="E25" s="29">
         <v>100</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="8">
         <v>1</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="8">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" ht="21" x14ac:dyDescent="0.3">
-      <c r="B26" s="25"/>
-      <c r="C26" s="13" t="s">
+      <c r="L25" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="M25" s="59"/>
+    </row>
+    <row r="26" spans="2:16" ht="26.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="21"/>
+      <c r="C26" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="32"/>
-      <c r="E26" s="9">
+      <c r="D26" s="28"/>
+      <c r="E26" s="8">
         <v>50</v>
       </c>
-      <c r="F26" s="34">
+      <c r="F26" s="30">
         <v>1</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="8">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" ht="21" x14ac:dyDescent="0.3">
-      <c r="B27" s="25"/>
-      <c r="C27" s="35" t="s">
+      <c r="L26" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M26" s="9"/>
+    </row>
+    <row r="27" spans="2:16" ht="21" x14ac:dyDescent="0.3">
+      <c r="B27" s="21"/>
+      <c r="C27" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="32"/>
-      <c r="E27" s="9">
+      <c r="D27" s="28"/>
+      <c r="E27" s="8">
         <v>20</v>
       </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="9">
+      <c r="F27" s="30"/>
+      <c r="G27" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="21" x14ac:dyDescent="0.3">
-      <c r="B28" s="25"/>
-      <c r="C28" s="13" t="s">
+    <row r="28" spans="2:16" ht="21" x14ac:dyDescent="0.3">
+      <c r="B28" s="21"/>
+      <c r="C28" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="9">
+      <c r="D28" s="28"/>
+      <c r="E28" s="8">
         <v>10</v>
       </c>
-      <c r="F28" s="34"/>
-      <c r="G28" s="9">
+      <c r="F28" s="30"/>
+      <c r="G28" s="8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" ht="21" x14ac:dyDescent="0.3">
-      <c r="B29" s="25"/>
-      <c r="C29" s="36" t="s">
+      <c r="L28" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="M28" s="60"/>
+    </row>
+    <row r="29" spans="2:16" ht="21" x14ac:dyDescent="0.3">
+      <c r="B29" s="21"/>
+      <c r="C29" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="32"/>
-      <c r="E29" s="37" t="s">
+      <c r="D29" s="28"/>
+      <c r="E29" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="38"/>
-      <c r="G29" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="25"/>
-      <c r="C30" s="13" t="s">
+      <c r="F29" s="34"/>
+      <c r="G29" s="8">
+        <v>0</v>
+      </c>
+      <c r="L29" s="60"/>
+      <c r="M29" s="60"/>
+    </row>
+    <row r="30" spans="2:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="21"/>
+      <c r="C30" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="39" t="s">
+      <c r="E30" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="40"/>
-      <c r="G30" s="41">
+      <c r="F30" s="36"/>
+      <c r="G30" s="37">
         <f>SUM(G22:G29)</f>
         <v>39650</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B31" s="25">
+    <row r="31" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="B31" s="21">
         <f>B20-B21-B22-B23-B24-B25-B26-B29-B30-B28-B27</f>
         <v>39949.199999999997</v>
       </c>
-      <c r="C31" s="42" t="s">
+      <c r="C31" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="43" t="s">
+      <c r="E31" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="43"/>
-      <c r="G31" s="44">
+      <c r="F31" s="49"/>
+      <c r="G31" s="39">
         <f>G30-B31</f>
         <v>-299.19999999999709</v>
       </c>
-      <c r="H31" s="8"/>
-    </row>
-    <row r="32" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B32" s="45"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="47">
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="2:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="B32" s="40"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42">
         <f>E32-F32</f>
         <v>0</v>
       </c>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="49" t="s">
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="4:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="D33" s="47">
+      <c r="D33" s="42">
         <f>D32*6</f>
         <v>0</v>
       </c>
@@ -1589,7 +1736,7 @@
       <c r="F33" s="50"/>
     </row>
     <row r="34" spans="4:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="D34" s="47">
+      <c r="D34" s="42">
         <f>B21-D33</f>
         <v>307</v>
       </c>
@@ -1600,7 +1747,9 @@
     </row>
     <row r="35" spans="4:6" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L29:M29"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E31:F31"/>

</xml_diff>